<commit_message>
Generate Report for Archive
</commit_message>
<xml_diff>
--- a/ol-handback/OpenLocalizationOrg/PowerShell-Docs/master/localization-status.xlsx
+++ b/ol-handback/OpenLocalizationOrg/PowerShell-Docs/master/localization-status.xlsx
@@ -466,6 +466,9 @@
     <t>2016-01-05 07:28:47</t>
   </si>
   <si>
+    <t>archiveResource.b4701b9fe5acf94be3fabf470371d8e47dd154d4.zh-cn.xlf</t>
+  </si>
+  <si>
     <t>authoringResource.106f1f4d77068b2b95f1927b611b5f405ec7a317.zh-cn.xlf</t>
   </si>
   <si>
@@ -598,6 +601,15 @@
     <t>serviceResource.17d839ef9952ec1a45ba971fcff47a80c41593cf.zh-cn.xlf</t>
   </si>
   <si>
+    <t>OpenLoc is cool.e253b4bff54b0434cc180a6770a453af141b2a53.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>SonjaFileToo.200fe5c96e02b06bc5f8a666c8090d57bedd4415.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>SonjaTest.bab99385ac372c3ae450ecdd8e590c3ad3219939.zh-cn.xlf</t>
+  </si>
+  <si>
     <t>TOC.b2a7935bce42ebc7e43bfe65f3058900e2942427.zh-cn.xlf</t>
   </si>
   <si>
@@ -614,18 +626,6 @@
   </si>
   <si>
     <t>README.8ec9a00bfd09b3190ac6b22251dbb1aa95a0579d.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>archiveResource.b4701b9fe5acf94be3fabf470371d8e47dd154d4.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>OpenLoc is cool.e253b4bff54b0434cc180a6770a453af141b2a53.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>SonjaFileToo.200fe5c96e02b06bc5f8a666c8090d57bedd4415.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>SonjaTest.bab99385ac372c3ae450ecdd8e590c3ad3219939.zh-cn.xlf</t>
   </si>
 </sst>
 </file>
@@ -786,7 +786,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>9</v>
@@ -982,7 +982,7 @@
         <v>5</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>24</v>
@@ -996,7 +996,7 @@
         <v>5</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>24</v>
@@ -1010,7 +1010,7 @@
         <v>5</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>24</v>
@@ -1024,7 +1024,7 @@
         <v>5</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>24</v>
@@ -1458,7 +1458,7 @@
         <v>5</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>59</v>
@@ -1472,7 +1472,7 @@
         <v>5</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>24</v>
@@ -1486,7 +1486,7 @@
         <v>5</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D53" s="2" t="s">
         <v>24</v>
@@ -3261,7 +3261,7 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>80</v>
@@ -3273,7 +3273,7 @@
         <v>150</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>149</v>
+        <v>9</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>82</v>
@@ -3284,7 +3284,7 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>80</v>
@@ -3296,7 +3296,7 @@
         <v>151</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>82</v>
@@ -3307,7 +3307,7 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>80</v>
@@ -3316,10 +3316,10 @@
         <v>6</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>153</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>152</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>82</v>
@@ -3330,7 +3330,7 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>80</v>
@@ -3342,7 +3342,7 @@
         <v>154</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>82</v>
@@ -3353,7 +3353,7 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>80</v>
@@ -3376,7 +3376,7 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>80</v>
@@ -3399,7 +3399,7 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>80</v>
@@ -3422,7 +3422,7 @@
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>80</v>
@@ -3445,7 +3445,7 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>80</v>
@@ -3468,7 +3468,7 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>80</v>
@@ -3491,7 +3491,7 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B13" s="0" t="s">
         <v>80</v>
@@ -3514,7 +3514,7 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B14" s="0" t="s">
         <v>80</v>
@@ -3537,7 +3537,7 @@
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B15" s="0" t="s">
         <v>80</v>
@@ -3560,7 +3560,7 @@
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B16" s="0" t="s">
         <v>80</v>
@@ -3583,99 +3583,111 @@
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>80</v>
+        <v>99</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>165</v>
+        <v>100</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>149</v>
+        <v>24</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>82</v>
       </c>
       <c r="J17" s="0" t="s">
-        <v>83</v>
+        <v>101</v>
+      </c>
+      <c r="K17" s="0" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>80</v>
+        <v>99</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>166</v>
+        <v>103</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>149</v>
+        <v>24</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>82</v>
       </c>
       <c r="J18" s="0" t="s">
-        <v>83</v>
+        <v>101</v>
+      </c>
+      <c r="K18" s="0" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>80</v>
+        <v>104</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>167</v>
+        <v>105</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>149</v>
+        <v>24</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>82</v>
       </c>
       <c r="J19" s="0" t="s">
-        <v>83</v>
+        <v>101</v>
+      </c>
+      <c r="K19" s="0" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>80</v>
+        <v>104</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>168</v>
+        <v>107</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>149</v>
+        <v>24</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>82</v>
       </c>
       <c r="J20" s="0" t="s">
-        <v>83</v>
+        <v>101</v>
+      </c>
+      <c r="K20" s="0" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B21" s="0" t="s">
         <v>80</v>
@@ -3684,7 +3696,7 @@
         <v>6</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>149</v>
@@ -3698,7 +3710,7 @@
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B22" s="0" t="s">
         <v>80</v>
@@ -3707,7 +3719,7 @@
         <v>6</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>149</v>
@@ -3721,7 +3733,7 @@
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B23" s="0" t="s">
         <v>80</v>
@@ -3730,7 +3742,7 @@
         <v>6</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>149</v>
@@ -3744,7 +3756,7 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B24" s="0" t="s">
         <v>80</v>
@@ -3753,7 +3765,7 @@
         <v>6</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>149</v>
@@ -3767,7 +3779,7 @@
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B25" s="0" t="s">
         <v>80</v>
@@ -3776,7 +3788,7 @@
         <v>6</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>149</v>
@@ -3790,7 +3802,7 @@
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B26" s="0" t="s">
         <v>80</v>
@@ -3799,7 +3811,7 @@
         <v>6</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>149</v>
@@ -3813,7 +3825,7 @@
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B27" s="0" t="s">
         <v>80</v>
@@ -3822,7 +3834,7 @@
         <v>6</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>149</v>
@@ -3836,7 +3848,7 @@
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B28" s="0" t="s">
         <v>80</v>
@@ -3845,7 +3857,7 @@
         <v>6</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>149</v>
@@ -3859,7 +3871,7 @@
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B29" s="0" t="s">
         <v>80</v>
@@ -3868,7 +3880,7 @@
         <v>6</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>149</v>
@@ -3882,7 +3894,7 @@
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B30" s="0" t="s">
         <v>80</v>
@@ -3891,7 +3903,7 @@
         <v>6</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>149</v>
@@ -3905,7 +3917,7 @@
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B31" s="0" t="s">
         <v>80</v>
@@ -3914,7 +3926,7 @@
         <v>6</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>149</v>
@@ -3928,7 +3940,7 @@
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B32" s="0" t="s">
         <v>80</v>
@@ -3937,7 +3949,7 @@
         <v>6</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>149</v>
@@ -3951,7 +3963,7 @@
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B33" s="0" t="s">
         <v>80</v>
@@ -3960,7 +3972,7 @@
         <v>6</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>149</v>
@@ -3974,7 +3986,7 @@
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B34" s="0" t="s">
         <v>80</v>
@@ -3983,7 +3995,7 @@
         <v>6</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>149</v>
@@ -3997,7 +4009,7 @@
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B35" s="0" t="s">
         <v>80</v>
@@ -4006,7 +4018,7 @@
         <v>6</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>149</v>
@@ -4020,7 +4032,7 @@
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B36" s="0" t="s">
         <v>80</v>
@@ -4029,7 +4041,7 @@
         <v>6</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>149</v>
@@ -4043,7 +4055,7 @@
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B37" s="0" t="s">
         <v>80</v>
@@ -4052,7 +4064,7 @@
         <v>6</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>149</v>
@@ -4066,7 +4078,7 @@
     </row>
     <row r="38">
       <c r="A38" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B38" s="0" t="s">
         <v>80</v>
@@ -4075,10 +4087,10 @@
         <v>6</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="H38" s="2" t="s">
         <v>82</v>
@@ -4089,7 +4101,7 @@
     </row>
     <row r="39">
       <c r="A39" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B39" s="0" t="s">
         <v>80</v>
@@ -4098,7 +4110,7 @@
         <v>6</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>149</v>
@@ -4112,7 +4124,7 @@
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B40" s="0" t="s">
         <v>80</v>
@@ -4121,7 +4133,7 @@
         <v>6</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>149</v>
@@ -4135,7 +4147,7 @@
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B41" s="0" t="s">
         <v>80</v>
@@ -4144,7 +4156,7 @@
         <v>6</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>149</v>
@@ -4158,7 +4170,7 @@
     </row>
     <row r="42">
       <c r="A42" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B42" s="0" t="s">
         <v>80</v>
@@ -4167,7 +4179,7 @@
         <v>6</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="E42" s="2" t="s">
         <v>149</v>
@@ -4181,7 +4193,7 @@
     </row>
     <row r="43">
       <c r="A43" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B43" s="0" t="s">
         <v>80</v>
@@ -4190,10 +4202,10 @@
         <v>6</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="H43" s="2" t="s">
         <v>82</v>
@@ -4204,7 +4216,7 @@
     </row>
     <row r="44">
       <c r="A44" s="1" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B44" s="0" t="s">
         <v>80</v>
@@ -4213,7 +4225,7 @@
         <v>6</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="E44" s="2" t="s">
         <v>149</v>
@@ -4227,7 +4239,7 @@
     </row>
     <row r="45">
       <c r="A45" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B45" s="0" t="s">
         <v>80</v>
@@ -4236,7 +4248,7 @@
         <v>6</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="E45" s="2" t="s">
         <v>149</v>
@@ -4250,7 +4262,7 @@
     </row>
     <row r="46">
       <c r="A46" s="1" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="B46" s="0" t="s">
         <v>80</v>
@@ -4259,7 +4271,7 @@
         <v>6</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>149</v>
@@ -4273,7 +4285,7 @@
     </row>
     <row r="47">
       <c r="A47" s="1" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="B47" s="0" t="s">
         <v>80</v>
@@ -4282,7 +4294,7 @@
         <v>6</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="E47" s="2" t="s">
         <v>149</v>
@@ -4296,7 +4308,7 @@
     </row>
     <row r="48">
       <c r="A48" s="1" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="B48" s="0" t="s">
         <v>80</v>
@@ -4305,7 +4317,7 @@
         <v>6</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E48" s="2" t="s">
         <v>149</v>
@@ -4319,7 +4331,7 @@
     </row>
     <row r="49">
       <c r="A49" s="1" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="B49" s="0" t="s">
         <v>80</v>
@@ -4328,7 +4340,7 @@
         <v>6</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="E49" s="2" t="s">
         <v>149</v>
@@ -4342,7 +4354,7 @@
     </row>
     <row r="50">
       <c r="A50" s="1" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="B50" s="0" t="s">
         <v>80</v>
@@ -4351,7 +4363,7 @@
         <v>6</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>149</v>
@@ -4365,7 +4377,7 @@
     </row>
     <row r="51">
       <c r="A51" s="1" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="B51" s="0" t="s">
         <v>80</v>
@@ -4374,10 +4386,10 @@
         <v>6</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>149</v>
+        <v>59</v>
       </c>
       <c r="H51" s="2" t="s">
         <v>82</v>
@@ -4388,19 +4400,19 @@
     </row>
     <row r="52">
       <c r="A52" s="1" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="B52" s="0" t="s">
         <v>80</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="H52" s="2" t="s">
         <v>82</v>
@@ -4411,16 +4423,16 @@
     </row>
     <row r="53">
       <c r="A53" s="1" t="s">
-        <v>23</v>
+        <v>61</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>99</v>
+        <v>80</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>100</v>
+        <v>197</v>
       </c>
       <c r="E53" s="2" t="s">
         <v>24</v>
@@ -4429,105 +4441,93 @@
         <v>82</v>
       </c>
       <c r="J53" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="K53" s="0" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="s">
-        <v>25</v>
+        <v>62</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>99</v>
+        <v>80</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>103</v>
+        <v>198</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>24</v>
+        <v>149</v>
       </c>
       <c r="H54" s="2" t="s">
         <v>82</v>
       </c>
       <c r="J54" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="K54" s="0" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="s">
-        <v>26</v>
+        <v>63</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>105</v>
+        <v>199</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>24</v>
+        <v>149</v>
       </c>
       <c r="H55" s="2" t="s">
         <v>82</v>
       </c>
       <c r="J55" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="K55" s="0" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="s">
-        <v>27</v>
+        <v>64</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>107</v>
+        <v>200</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>24</v>
+        <v>149</v>
       </c>
       <c r="H56" s="2" t="s">
         <v>82</v>
       </c>
       <c r="J56" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="K56" s="0" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="B57" s="0" t="s">
         <v>80</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>201</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>59</v>
+        <v>149</v>
       </c>
       <c r="H57" s="2" t="s">
         <v>82</v>
@@ -4538,19 +4538,19 @@
     </row>
     <row r="58">
       <c r="A58" s="1" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="B58" s="0" t="s">
         <v>80</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>202</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>24</v>
+        <v>149</v>
       </c>
       <c r="H58" s="2" t="s">
         <v>82</v>
@@ -4561,19 +4561,19 @@
     </row>
     <row r="59">
       <c r="A59" s="1" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="B59" s="0" t="s">
         <v>80</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>203</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>24</v>
+        <v>149</v>
       </c>
       <c r="H59" s="2" t="s">
         <v>82</v>
@@ -4586,120 +4586,120 @@
   <hyperlinks>
     <hyperlink ref="A2" display="CONTRIBUTING.md" r:id="rId2"/>
     <hyperlink ref="D2" display="CONTRIBUTING.3f454a98e586d1aa0d322e19afd5e67e08f2d3c8.zh-cn.xlf" r:id="rId3"/>
-    <hyperlink ref="A3" display="authoringResource.md" r:id="rId4"/>
-    <hyperlink ref="D3" display="authoringResource.106f1f4d77068b2b95f1927b611b5f405ec7a317.zh-cn.xlf" r:id="rId5"/>
-    <hyperlink ref="A4" display="authoringResourceClass.md" r:id="rId6"/>
-    <hyperlink ref="D4" display="authoringResourceClass.3603134df9ad1cad202d10769ff631a083cc3aae.zh-cn.xlf" r:id="rId7"/>
-    <hyperlink ref="A5" display="authoringResourceComposite.md" r:id="rId8"/>
-    <hyperlink ref="D5" display="authoringResourceComposite.6d5d1e53e83e25cfc63e26078da390a4fa6737f2.zh-cn.xlf" r:id="rId9"/>
-    <hyperlink ref="A6" display="authoringResourceMOF.md" r:id="rId10"/>
-    <hyperlink ref="D6" display="authoringResourceMOF.1f503c33425780c369e78193e2f2f4e9242c401b.zh-cn.xlf" r:id="rId11"/>
-    <hyperlink ref="A7" display="authoringResourceMofCS.md" r:id="rId12"/>
-    <hyperlink ref="D7" display="authoringResourceMofCS.0647b27b00ec52b2f524a2856e48bc7c29c0f867.zh-cn.xlf" r:id="rId13"/>
-    <hyperlink ref="A8" display="authoringResourceMofDesigner.md" r:id="rId14"/>
-    <hyperlink ref="D8" display="authoringResourceMofDesigner.09b1adffc4afb0d9b1154880e2dab0b25d82d51b.zh-cn.xlf" r:id="rId15"/>
-    <hyperlink ref="A9" display="builtInResource.md" r:id="rId16"/>
-    <hyperlink ref="D9" display="builtInResource.2f855e1582347e986aa4e5e62b842b886596fdc2.zh-cn.xlf" r:id="rId17"/>
-    <hyperlink ref="A10" display="configData.md" r:id="rId18"/>
-    <hyperlink ref="D10" display="configData.51d01a46dd9af8b425788cc485523b09f8470b95.zh-cn.xlf" r:id="rId19"/>
-    <hyperlink ref="A11" display="configurations.md" r:id="rId20"/>
-    <hyperlink ref="D11" display="configurations.02626ddbf3a00f8ede56fdfd2e46a027800e75b6.zh-cn.xlf" r:id="rId21"/>
-    <hyperlink ref="A12" display="enactingConfigurations.md" r:id="rId22"/>
-    <hyperlink ref="D12" display="enactingConfigurations.5949c3926cc7d368fa49b0ba340a078984794e5d.zh-cn.xlf" r:id="rId23"/>
-    <hyperlink ref="A13" display="environmentResource.md" r:id="rId24"/>
-    <hyperlink ref="D13" display="environmentResource.eb91ffd4cd8bdb9476e5a83de1a20d3b7b502a56.zh-cn.xlf" r:id="rId25"/>
-    <hyperlink ref="A14" display="fileResource.md" r:id="rId26"/>
-    <hyperlink ref="D14" display="fileResource.ad0d9bba41b615db808e5dfc814b50945863b3da.zh-cn.xlf" r:id="rId27"/>
-    <hyperlink ref="A15" display="groupResource.md" r:id="rId28"/>
-    <hyperlink ref="D15" display="groupResource.d19d416269795c92566b62c36b9782062dcea43e.zh-cn.xlf" r:id="rId29"/>
-    <hyperlink ref="A16" display="lnxArchiveResource.md" r:id="rId30"/>
-    <hyperlink ref="D16" display="lnxArchiveResource.095aab7d23720fd394f2573c30223a6bbcc0a4ef.zh-cn.xlf" r:id="rId31"/>
-    <hyperlink ref="A17" display="lnxBuiltInResources.md" r:id="rId32"/>
-    <hyperlink ref="D17" display="lnxBuiltInResources.12cc0e2a7d17afe6b1e1b9c928760080863926f9.zh-cn.xlf" r:id="rId33"/>
-    <hyperlink ref="A18" display="lnxEnvironmentResource.md" r:id="rId34"/>
-    <hyperlink ref="D18" display="lnxEnvironmentResource.60c6523b1d06708f748c9039105a2042fa341552.zh-cn.xlf" r:id="rId35"/>
-    <hyperlink ref="A19" display="lnxFileLineResource.md" r:id="rId36"/>
-    <hyperlink ref="D19" display="lnxFileLineResource.d91fc802a4c6cdbff5a2e35f92b34c36c6dbf5eb.zh-cn.xlf" r:id="rId37"/>
-    <hyperlink ref="A20" display="lnxFileResource.md" r:id="rId38"/>
-    <hyperlink ref="D20" display="lnxFileResource.1f67ed46e7bb4ac04f73143e1d7ab7e9199d3191.zh-cn.xlf" r:id="rId39"/>
-    <hyperlink ref="A21" display="lnxGettingStarted.md" r:id="rId40"/>
-    <hyperlink ref="D21" display="lnxGettingStarted.1601cf6d0eb8b4f7343575c8fbf2106bfaad8b65.zh-cn.xlf" r:id="rId41"/>
-    <hyperlink ref="A22" display="lnxGroupResource.md" r:id="rId42"/>
-    <hyperlink ref="D22" display="lnxGroupResource.0cedb684d797032bd47cdb852629c36da0884567.zh-cn.xlf" r:id="rId43"/>
-    <hyperlink ref="A23" display="lnxPackageResource.md" r:id="rId44"/>
-    <hyperlink ref="D23" display="lnxPackageResource.db35ab938bbfbb38cae53fe9ae98fd22b5f18009.zh-cn.xlf" r:id="rId45"/>
-    <hyperlink ref="A24" display="lnxScriptResource.md" r:id="rId46"/>
-    <hyperlink ref="D24" display="lnxScriptResource.1344a5d5b807ee53705e93842d9ef5e25a883359.zh-cn.xlf" r:id="rId47"/>
-    <hyperlink ref="A25" display="lnxServiceResource.md" r:id="rId48"/>
-    <hyperlink ref="D25" display="lnxServiceResource.e637c7f7b18939ec8c16eadf2c42ab00e236fb7b.zh-cn.xlf" r:id="rId49"/>
-    <hyperlink ref="A26" display="lnxSshAuthorizedKeysResource.md" r:id="rId50"/>
-    <hyperlink ref="D26" display="lnxSshAuthorizedKeysResource.9a647ff238cd38a2fc7da58f3cc5682acf7d3346.zh-cn.xlf" r:id="rId51"/>
-    <hyperlink ref="A27" display="lnxUserResource.md" r:id="rId52"/>
-    <hyperlink ref="D27" display="lnxUserResource.2376554a25dd8dfad6a78a6180b7c7166e4817e1.zh-cn.xlf" r:id="rId53"/>
-    <hyperlink ref="A28" display="logResource.md" r:id="rId54"/>
-    <hyperlink ref="D28" display="logResource.07af9dfcf6076ef19059178c3b404762677920f0.zh-cn.xlf" r:id="rId55"/>
-    <hyperlink ref="A29" display="metaConfig.md" r:id="rId56"/>
-    <hyperlink ref="D29" display="metaConfig.915dba9ed66671e4a41c35a16d5248bb4c94e3d6.zh-cn.xlf" r:id="rId57"/>
-    <hyperlink ref="A30" display="metaConfig4.md" r:id="rId58"/>
-    <hyperlink ref="D30" display="metaConfig4.4ec702d458e6574099cead724f0e57c3c5d262df.zh-cn.xlf" r:id="rId59"/>
-    <hyperlink ref="A31" display="overview.md" r:id="rId60"/>
-    <hyperlink ref="D31" display="overview.8cc85dd99239e10c76baa6006d906abfd6122c3f.zh-cn.xlf" r:id="rId61"/>
-    <hyperlink ref="A32" display="packageResource.md" r:id="rId62"/>
-    <hyperlink ref="D32" display="packageResource.132c4949cee174dc0dc324456d220436cb9884e6.zh-cn.xlf" r:id="rId63"/>
-    <hyperlink ref="A33" display="partialConfigs.md" r:id="rId64"/>
-    <hyperlink ref="D33" display="partialConfigs.f483ab7fa1511b557780a02b5b807245f730c1b6.zh-cn.xlf" r:id="rId65"/>
-    <hyperlink ref="A34" display="pullClient.md" r:id="rId66"/>
-    <hyperlink ref="D34" display="pullClient.4844144e7d40a6e8b1be2cfaa80a5307f19f47f9.zh-cn.xlf" r:id="rId67"/>
-    <hyperlink ref="A35" display="pullClientConfigID.md" r:id="rId68"/>
-    <hyperlink ref="D35" display="pullClientConfigID.1b955603d220e49bbe52711bacf74c46feec04cc.zh-cn.xlf" r:id="rId69"/>
-    <hyperlink ref="A36" display="pullClientConfigID4.md" r:id="rId70"/>
-    <hyperlink ref="D36" display="pullClientConfigID4.3556f8028eee8a539990f2895506bcbafb14a012.zh-cn.xlf" r:id="rId71"/>
-    <hyperlink ref="A37" display="pullClientConfigNames.md" r:id="rId72"/>
-    <hyperlink ref="D37" display="pullClientConfigNames.90531abb3b29bfd751ad2f3a115a4ba02024827e.zh-cn.xlf" r:id="rId73"/>
-    <hyperlink ref="A38" display="pullServer.md" r:id="rId74"/>
-    <hyperlink ref="D38" display="pullServer.4b925b277da29998394af746bdbdd508fda48909.zh-cn.xlf" r:id="rId75"/>
-    <hyperlink ref="A39" display="queryServerNodes.md" r:id="rId76"/>
-    <hyperlink ref="D39" display="queryServerNodes.bb63da39c46de8db127c93721dcbec9b10f73d2d.zh-cn.xlf" r:id="rId77"/>
-    <hyperlink ref="A40" display="registryResource.md" r:id="rId78"/>
-    <hyperlink ref="D40" display="registryResource.7e5e3fabff013c107bd112ac774a50c9cab7c90a.zh-cn.xlf" r:id="rId79"/>
-    <hyperlink ref="A41" display="resources.md" r:id="rId80"/>
-    <hyperlink ref="D41" display="resources.41990b4bc17648676f43a9aedfa72aa3db455ca3.zh-cn.xlf" r:id="rId81"/>
-    <hyperlink ref="A42" display="scriptResource.md" r:id="rId82"/>
-    <hyperlink ref="D42" display="scriptResource.086a4e23c7f1950435cf115060757fcd9b7f7f5d.zh-cn.xlf" r:id="rId83"/>
-    <hyperlink ref="A43" display="secureMOF.md" r:id="rId84"/>
-    <hyperlink ref="D43" display="secureMOF.84bae90620632fc30568f4afa595e2b86e8aa6d1.zh-cn.xlf" r:id="rId85"/>
-    <hyperlink ref="A44" display="secureServer.md" r:id="rId86"/>
-    <hyperlink ref="D44" display="secureServer.ce207607010d18109152742ba23c923cd3cddba2.zh-cn.xlf" r:id="rId87"/>
-    <hyperlink ref="A45" display="serviceResource.md" r:id="rId88"/>
-    <hyperlink ref="D45" display="serviceResource.17d839ef9952ec1a45ba971fcff47a80c41593cf.zh-cn.xlf" r:id="rId89"/>
-    <hyperlink ref="A46" display="TOC.md" r:id="rId90"/>
-    <hyperlink ref="D46" display="TOC.b2a7935bce42ebc7e43bfe65f3058900e2942427.zh-cn.xlf" r:id="rId91"/>
-    <hyperlink ref="A47" display="troubleshooting.md" r:id="rId92"/>
-    <hyperlink ref="D47" display="troubleshooting.bcb1039de4ec46bfb0ab2d224be50829d0891e7d.zh-cn.xlf" r:id="rId93"/>
-    <hyperlink ref="A48" display="userResource.md" r:id="rId94"/>
-    <hyperlink ref="D48" display="userResource.5de4fbe03e9e06934442ba451eb0564931863f45.zh-cn.xlf" r:id="rId95"/>
-    <hyperlink ref="A49" display="windowsfeatureResource.md" r:id="rId96"/>
-    <hyperlink ref="D49" display="windowsfeatureResource.07b968eb71ba947a4bf5fa25add8a0e2c25bcadf.zh-cn.xlf" r:id="rId97"/>
-    <hyperlink ref="A50" display="windowsProcessResource.md" r:id="rId98"/>
-    <hyperlink ref="D50" display="windowsProcessResource.d5014f2fde06deea365cd1e64a3587c037999fa7.zh-cn.xlf" r:id="rId99"/>
-    <hyperlink ref="A51" display="README.md" r:id="rId100"/>
-    <hyperlink ref="D51" display="README.8ec9a00bfd09b3190ac6b22251dbb1aa95a0579d.zh-cn.xlf" r:id="rId101"/>
-    <hyperlink ref="A52" display="archiveResource.md" r:id="rId102"/>
-    <hyperlink ref="D52" display="archiveResource.b4701b9fe5acf94be3fabf470371d8e47dd154d4.zh-cn.xlf" r:id="rId103"/>
-    <hyperlink ref="A53" display="PartialConfig1.jpg" r:id="rId104"/>
-    <hyperlink ref="D53" display="3e61149f7b05f74d662d3038233013ffdcbed1a3.jpg" r:id="rId105"/>
-    <hyperlink ref="A54" display="PartialConfigPullServer.jpg" r:id="rId106"/>
-    <hyperlink ref="D54" display="1ba842005c2b1ce80a3670429b3e010c7b1c1f59.jpg" r:id="rId107"/>
-    <hyperlink ref="A55" display="Pull.png" r:id="rId108"/>
-    <hyperlink ref="D55" display="86d829b1fcdd41e648ed0594eaf337b3726c143c.png" r:id="rId109"/>
-    <hyperlink ref="A56" display="Push.png" r:id="rId110"/>
-    <hyperlink ref="D56" display="d3008e3fe7da4c118c693d2b34a0b329780f8d86.png" r:id="rId111"/>
-    <hyperlink ref="A57" display="OpenLoc is cool.md" r:id="rId112"/>
-    <hyperlink ref="D57" display="OpenLoc is cool.e253b4bff54b0434cc180a6770a453af141b2a53.zh-cn.xlf" r:id="rId113"/>
-    <hyperlink ref="A58" display="SonjaFileToo.md" r:id="rId114"/>
-    <hyperlink ref="D58" display="SonjaFileToo.200fe5c96e02b06bc5f8a666c8090d57bedd4415.zh-cn.xlf" r:id="rId115"/>
-    <hyperlink ref="A59" display="SonjaTest.md" r:id="rId116"/>
-    <hyperlink ref="D59" display="SonjaTest.bab99385ac372c3ae450ecdd8e590c3ad3219939.zh-cn.xlf" r:id="rId117"/>
+    <hyperlink ref="A3" display="archiveResource.md" r:id="rId4"/>
+    <hyperlink ref="D3" display="archiveResource.b4701b9fe5acf94be3fabf470371d8e47dd154d4.zh-cn.xlf" r:id="rId5"/>
+    <hyperlink ref="A4" display="authoringResource.md" r:id="rId6"/>
+    <hyperlink ref="D4" display="authoringResource.106f1f4d77068b2b95f1927b611b5f405ec7a317.zh-cn.xlf" r:id="rId7"/>
+    <hyperlink ref="A5" display="authoringResourceClass.md" r:id="rId8"/>
+    <hyperlink ref="D5" display="authoringResourceClass.3603134df9ad1cad202d10769ff631a083cc3aae.zh-cn.xlf" r:id="rId9"/>
+    <hyperlink ref="A6" display="authoringResourceComposite.md" r:id="rId10"/>
+    <hyperlink ref="D6" display="authoringResourceComposite.6d5d1e53e83e25cfc63e26078da390a4fa6737f2.zh-cn.xlf" r:id="rId11"/>
+    <hyperlink ref="A7" display="authoringResourceMOF.md" r:id="rId12"/>
+    <hyperlink ref="D7" display="authoringResourceMOF.1f503c33425780c369e78193e2f2f4e9242c401b.zh-cn.xlf" r:id="rId13"/>
+    <hyperlink ref="A8" display="authoringResourceMofCS.md" r:id="rId14"/>
+    <hyperlink ref="D8" display="authoringResourceMofCS.0647b27b00ec52b2f524a2856e48bc7c29c0f867.zh-cn.xlf" r:id="rId15"/>
+    <hyperlink ref="A9" display="authoringResourceMofDesigner.md" r:id="rId16"/>
+    <hyperlink ref="D9" display="authoringResourceMofDesigner.09b1adffc4afb0d9b1154880e2dab0b25d82d51b.zh-cn.xlf" r:id="rId17"/>
+    <hyperlink ref="A10" display="builtInResource.md" r:id="rId18"/>
+    <hyperlink ref="D10" display="builtInResource.2f855e1582347e986aa4e5e62b842b886596fdc2.zh-cn.xlf" r:id="rId19"/>
+    <hyperlink ref="A11" display="configData.md" r:id="rId20"/>
+    <hyperlink ref="D11" display="configData.51d01a46dd9af8b425788cc485523b09f8470b95.zh-cn.xlf" r:id="rId21"/>
+    <hyperlink ref="A12" display="configurations.md" r:id="rId22"/>
+    <hyperlink ref="D12" display="configurations.02626ddbf3a00f8ede56fdfd2e46a027800e75b6.zh-cn.xlf" r:id="rId23"/>
+    <hyperlink ref="A13" display="enactingConfigurations.md" r:id="rId24"/>
+    <hyperlink ref="D13" display="enactingConfigurations.5949c3926cc7d368fa49b0ba340a078984794e5d.zh-cn.xlf" r:id="rId25"/>
+    <hyperlink ref="A14" display="environmentResource.md" r:id="rId26"/>
+    <hyperlink ref="D14" display="environmentResource.eb91ffd4cd8bdb9476e5a83de1a20d3b7b502a56.zh-cn.xlf" r:id="rId27"/>
+    <hyperlink ref="A15" display="fileResource.md" r:id="rId28"/>
+    <hyperlink ref="D15" display="fileResource.ad0d9bba41b615db808e5dfc814b50945863b3da.zh-cn.xlf" r:id="rId29"/>
+    <hyperlink ref="A16" display="groupResource.md" r:id="rId30"/>
+    <hyperlink ref="D16" display="groupResource.d19d416269795c92566b62c36b9782062dcea43e.zh-cn.xlf" r:id="rId31"/>
+    <hyperlink ref="A17" display="PartialConfig1.jpg" r:id="rId32"/>
+    <hyperlink ref="D17" display="3e61149f7b05f74d662d3038233013ffdcbed1a3.jpg" r:id="rId33"/>
+    <hyperlink ref="A18" display="PartialConfigPullServer.jpg" r:id="rId34"/>
+    <hyperlink ref="D18" display="1ba842005c2b1ce80a3670429b3e010c7b1c1f59.jpg" r:id="rId35"/>
+    <hyperlink ref="A19" display="Pull.png" r:id="rId36"/>
+    <hyperlink ref="D19" display="86d829b1fcdd41e648ed0594eaf337b3726c143c.png" r:id="rId37"/>
+    <hyperlink ref="A20" display="Push.png" r:id="rId38"/>
+    <hyperlink ref="D20" display="d3008e3fe7da4c118c693d2b34a0b329780f8d86.png" r:id="rId39"/>
+    <hyperlink ref="A21" display="lnxArchiveResource.md" r:id="rId40"/>
+    <hyperlink ref="D21" display="lnxArchiveResource.095aab7d23720fd394f2573c30223a6bbcc0a4ef.zh-cn.xlf" r:id="rId41"/>
+    <hyperlink ref="A22" display="lnxBuiltInResources.md" r:id="rId42"/>
+    <hyperlink ref="D22" display="lnxBuiltInResources.12cc0e2a7d17afe6b1e1b9c928760080863926f9.zh-cn.xlf" r:id="rId43"/>
+    <hyperlink ref="A23" display="lnxEnvironmentResource.md" r:id="rId44"/>
+    <hyperlink ref="D23" display="lnxEnvironmentResource.60c6523b1d06708f748c9039105a2042fa341552.zh-cn.xlf" r:id="rId45"/>
+    <hyperlink ref="A24" display="lnxFileLineResource.md" r:id="rId46"/>
+    <hyperlink ref="D24" display="lnxFileLineResource.d91fc802a4c6cdbff5a2e35f92b34c36c6dbf5eb.zh-cn.xlf" r:id="rId47"/>
+    <hyperlink ref="A25" display="lnxFileResource.md" r:id="rId48"/>
+    <hyperlink ref="D25" display="lnxFileResource.1f67ed46e7bb4ac04f73143e1d7ab7e9199d3191.zh-cn.xlf" r:id="rId49"/>
+    <hyperlink ref="A26" display="lnxGettingStarted.md" r:id="rId50"/>
+    <hyperlink ref="D26" display="lnxGettingStarted.1601cf6d0eb8b4f7343575c8fbf2106bfaad8b65.zh-cn.xlf" r:id="rId51"/>
+    <hyperlink ref="A27" display="lnxGroupResource.md" r:id="rId52"/>
+    <hyperlink ref="D27" display="lnxGroupResource.0cedb684d797032bd47cdb852629c36da0884567.zh-cn.xlf" r:id="rId53"/>
+    <hyperlink ref="A28" display="lnxPackageResource.md" r:id="rId54"/>
+    <hyperlink ref="D28" display="lnxPackageResource.db35ab938bbfbb38cae53fe9ae98fd22b5f18009.zh-cn.xlf" r:id="rId55"/>
+    <hyperlink ref="A29" display="lnxScriptResource.md" r:id="rId56"/>
+    <hyperlink ref="D29" display="lnxScriptResource.1344a5d5b807ee53705e93842d9ef5e25a883359.zh-cn.xlf" r:id="rId57"/>
+    <hyperlink ref="A30" display="lnxServiceResource.md" r:id="rId58"/>
+    <hyperlink ref="D30" display="lnxServiceResource.e637c7f7b18939ec8c16eadf2c42ab00e236fb7b.zh-cn.xlf" r:id="rId59"/>
+    <hyperlink ref="A31" display="lnxSshAuthorizedKeysResource.md" r:id="rId60"/>
+    <hyperlink ref="D31" display="lnxSshAuthorizedKeysResource.9a647ff238cd38a2fc7da58f3cc5682acf7d3346.zh-cn.xlf" r:id="rId61"/>
+    <hyperlink ref="A32" display="lnxUserResource.md" r:id="rId62"/>
+    <hyperlink ref="D32" display="lnxUserResource.2376554a25dd8dfad6a78a6180b7c7166e4817e1.zh-cn.xlf" r:id="rId63"/>
+    <hyperlink ref="A33" display="logResource.md" r:id="rId64"/>
+    <hyperlink ref="D33" display="logResource.07af9dfcf6076ef19059178c3b404762677920f0.zh-cn.xlf" r:id="rId65"/>
+    <hyperlink ref="A34" display="metaConfig.md" r:id="rId66"/>
+    <hyperlink ref="D34" display="metaConfig.915dba9ed66671e4a41c35a16d5248bb4c94e3d6.zh-cn.xlf" r:id="rId67"/>
+    <hyperlink ref="A35" display="metaConfig4.md" r:id="rId68"/>
+    <hyperlink ref="D35" display="metaConfig4.4ec702d458e6574099cead724f0e57c3c5d262df.zh-cn.xlf" r:id="rId69"/>
+    <hyperlink ref="A36" display="overview.md" r:id="rId70"/>
+    <hyperlink ref="D36" display="overview.8cc85dd99239e10c76baa6006d906abfd6122c3f.zh-cn.xlf" r:id="rId71"/>
+    <hyperlink ref="A37" display="packageResource.md" r:id="rId72"/>
+    <hyperlink ref="D37" display="packageResource.132c4949cee174dc0dc324456d220436cb9884e6.zh-cn.xlf" r:id="rId73"/>
+    <hyperlink ref="A38" display="partialConfigs.md" r:id="rId74"/>
+    <hyperlink ref="D38" display="partialConfigs.f483ab7fa1511b557780a02b5b807245f730c1b6.zh-cn.xlf" r:id="rId75"/>
+    <hyperlink ref="A39" display="pullClient.md" r:id="rId76"/>
+    <hyperlink ref="D39" display="pullClient.4844144e7d40a6e8b1be2cfaa80a5307f19f47f9.zh-cn.xlf" r:id="rId77"/>
+    <hyperlink ref="A40" display="pullClientConfigID.md" r:id="rId78"/>
+    <hyperlink ref="D40" display="pullClientConfigID.1b955603d220e49bbe52711bacf74c46feec04cc.zh-cn.xlf" r:id="rId79"/>
+    <hyperlink ref="A41" display="pullClientConfigID4.md" r:id="rId80"/>
+    <hyperlink ref="D41" display="pullClientConfigID4.3556f8028eee8a539990f2895506bcbafb14a012.zh-cn.xlf" r:id="rId81"/>
+    <hyperlink ref="A42" display="pullClientConfigNames.md" r:id="rId82"/>
+    <hyperlink ref="D42" display="pullClientConfigNames.90531abb3b29bfd751ad2f3a115a4ba02024827e.zh-cn.xlf" r:id="rId83"/>
+    <hyperlink ref="A43" display="pullServer.md" r:id="rId84"/>
+    <hyperlink ref="D43" display="pullServer.4b925b277da29998394af746bdbdd508fda48909.zh-cn.xlf" r:id="rId85"/>
+    <hyperlink ref="A44" display="queryServerNodes.md" r:id="rId86"/>
+    <hyperlink ref="D44" display="queryServerNodes.bb63da39c46de8db127c93721dcbec9b10f73d2d.zh-cn.xlf" r:id="rId87"/>
+    <hyperlink ref="A45" display="registryResource.md" r:id="rId88"/>
+    <hyperlink ref="D45" display="registryResource.7e5e3fabff013c107bd112ac774a50c9cab7c90a.zh-cn.xlf" r:id="rId89"/>
+    <hyperlink ref="A46" display="resources.md" r:id="rId90"/>
+    <hyperlink ref="D46" display="resources.41990b4bc17648676f43a9aedfa72aa3db455ca3.zh-cn.xlf" r:id="rId91"/>
+    <hyperlink ref="A47" display="scriptResource.md" r:id="rId92"/>
+    <hyperlink ref="D47" display="scriptResource.086a4e23c7f1950435cf115060757fcd9b7f7f5d.zh-cn.xlf" r:id="rId93"/>
+    <hyperlink ref="A48" display="secureMOF.md" r:id="rId94"/>
+    <hyperlink ref="D48" display="secureMOF.84bae90620632fc30568f4afa595e2b86e8aa6d1.zh-cn.xlf" r:id="rId95"/>
+    <hyperlink ref="A49" display="secureServer.md" r:id="rId96"/>
+    <hyperlink ref="D49" display="secureServer.ce207607010d18109152742ba23c923cd3cddba2.zh-cn.xlf" r:id="rId97"/>
+    <hyperlink ref="A50" display="serviceResource.md" r:id="rId98"/>
+    <hyperlink ref="D50" display="serviceResource.17d839ef9952ec1a45ba971fcff47a80c41593cf.zh-cn.xlf" r:id="rId99"/>
+    <hyperlink ref="A51" display="OpenLoc is cool.md" r:id="rId100"/>
+    <hyperlink ref="D51" display="OpenLoc is cool.e253b4bff54b0434cc180a6770a453af141b2a53.zh-cn.xlf" r:id="rId101"/>
+    <hyperlink ref="A52" display="SonjaFileToo.md" r:id="rId102"/>
+    <hyperlink ref="D52" display="SonjaFileToo.200fe5c96e02b06bc5f8a666c8090d57bedd4415.zh-cn.xlf" r:id="rId103"/>
+    <hyperlink ref="A53" display="SonjaTest.md" r:id="rId104"/>
+    <hyperlink ref="D53" display="SonjaTest.bab99385ac372c3ae450ecdd8e590c3ad3219939.zh-cn.xlf" r:id="rId105"/>
+    <hyperlink ref="A54" display="TOC.md" r:id="rId106"/>
+    <hyperlink ref="D54" display="TOC.b2a7935bce42ebc7e43bfe65f3058900e2942427.zh-cn.xlf" r:id="rId107"/>
+    <hyperlink ref="A55" display="troubleshooting.md" r:id="rId108"/>
+    <hyperlink ref="D55" display="troubleshooting.bcb1039de4ec46bfb0ab2d224be50829d0891e7d.zh-cn.xlf" r:id="rId109"/>
+    <hyperlink ref="A56" display="userResource.md" r:id="rId110"/>
+    <hyperlink ref="D56" display="userResource.5de4fbe03e9e06934442ba451eb0564931863f45.zh-cn.xlf" r:id="rId111"/>
+    <hyperlink ref="A57" display="windowsfeatureResource.md" r:id="rId112"/>
+    <hyperlink ref="D57" display="windowsfeatureResource.07b968eb71ba947a4bf5fa25add8a0e2c25bcadf.zh-cn.xlf" r:id="rId113"/>
+    <hyperlink ref="A58" display="windowsProcessResource.md" r:id="rId114"/>
+    <hyperlink ref="D58" display="windowsProcessResource.d5014f2fde06deea365cd1e64a3587c037999fa7.zh-cn.xlf" r:id="rId115"/>
+    <hyperlink ref="A59" display="README.md" r:id="rId116"/>
+    <hyperlink ref="D59" display="README.8ec9a00bfd09b3190ac6b22251dbb1aa95a0579d.zh-cn.xlf" r:id="rId117"/>
   </hyperlinks>
   <headerFooter/>
   <tableParts>

</xml_diff>